<commit_message>
Atualização automática do arquivo Excel
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -692,6 +692,191 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Globo</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Bom Dia Brasil</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cultura</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-03-28T15:57</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Neutro</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Sem Nota</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Globo</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Bom Dia Rio</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Codemca</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-03-28T15:57</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Neutro</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Sem Nota</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>teste2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Record</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Balanço Geral</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Codemca</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-03-14T16:08</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Neutro</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Com Nota</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Globo</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Inter TV Rural</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Agricultura</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-03-28T18:11</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Neutro</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Sem Nota</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaaaaaaaaaaateste3333333</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Globo</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Inter TV Rural</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cultura</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-03-28T16:12</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Neutro</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Com Nota</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>212121212</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>